<commit_message>
Fixed Efficiecy and Output
</commit_message>
<xml_diff>
--- a/sheet.xlsx
+++ b/sheet.xlsx
@@ -2,6 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rates" sheetId="2" state="visible" r:id="rId2"/>
@@ -13,21 +16,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="3">
     <font>
-      <name val="Arial"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="Arial"/>
-      <color theme="1"/>
-      <scheme val="minor"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -38,11 +42,24 @@
       <patternFill/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin"/>
       <right style="thin"/>
@@ -51,22 +68,33 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -139,14 +167,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -173,22 +201,82 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -200,153 +288,188 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="18" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>FromCurrency</t>
@@ -357,18 +480,18 @@
           <t>ToCurrency</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>FromDate</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>ToDate</t>
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="18" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>INR</t>
@@ -386,7 +509,7 @@
         <v>45467</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="18" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>USD</t>
@@ -404,7 +527,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="18" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>EUR</t>
@@ -422,7 +545,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="18" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>INR</t>
@@ -441,7 +564,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -460,506 +583,506 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>FromCurrency</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>ToCurrency</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Rate</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>FromCurrency</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>ToCurrency</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>2024-06-20</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>85.175015</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
         <is>
           <t>2024-06-21</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>85.375955</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
         <is>
           <t>2024-06-22</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>85.350455</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
         <is>
           <t>2024-06-23</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>85.350455</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
         <is>
           <t>2024-06-24</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>85.350455</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>2023-12-01</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>1.120571</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
         <is>
           <t>2023-12-02</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>1.113329</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
         <is>
           <t>2023-12-03</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>1.113329</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
         <is>
           <t>2023-12-04</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>1.113329</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
         <is>
           <t>2023-12-05</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>1.111493</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
         <is>
           <t>2023-12-06</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>1.106699</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
         <is>
           <t>2023-12-07</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>1.102211</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
         <is>
           <t>2023-12-08</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>1.103537</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
         <is>
           <t>2023-12-09</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>1.101905</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
         <is>
           <t>2023-12-10</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>1.101905</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>2024-01-10</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>0.011263</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
         <is>
           <t>2024-01-11</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>0.011261</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
         <is>
           <t>2024-01-12</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>0.011256</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
         <is>
           <t>2024-01-13</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>0.011259</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
         <is>
           <t>2024-01-14</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>0.011259</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
         <is>
           <t>2024-01-15</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>0.011259</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>JPY</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>2024-05-10</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>0.549221</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>JPY</t>
-        </is>
-      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
         <is>
           <t>2024-05-11</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>0.549146</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
         <is>
           <t>2024-05-12</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>0.549146</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
         <is>
           <t>2024-05-13</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>0.549146</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
         <is>
           <t>2024-05-14</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>0.548182</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
         <is>
           <t>2024-05-15</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>0.545937</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
         <is>
           <t>2024-05-16</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>0.550844</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
         <is>
           <t>2024-05-17</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>0.554892</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
         <is>
           <t>2024-05-18</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>0.548918</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
         <is>
           <t>2024-05-19</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>0.548918</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
         <is>
           <t>2024-05-20</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>0.548918</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>